<commit_message>
updates results ammonia kits
</commit_message>
<xml_diff>
--- a/Incubations/Results/ammonia kits.xlsx
+++ b/Incubations/Results/ammonia kits.xlsx
@@ -5,16 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patriciatran/Dropbox/McMahonLab_Project/Nitrogen_Project/Metagenome/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patriciatran/Documents/GitHub/Nitrogen_Project/Incubations/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16560" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16560" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="180227_results" sheetId="1" r:id="rId1"/>
+    <sheet name="180228_results" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,50 +28,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="46">
   <si>
     <t>SampleID</t>
   </si>
   <si>
-    <t>Reading_nm</t>
-  </si>
-  <si>
-    <t>MEDH_5A</t>
-  </si>
-  <si>
-    <t>MEDH_5B</t>
-  </si>
-  <si>
-    <t>MEDH_10A</t>
-  </si>
-  <si>
-    <t>MEDH_10B</t>
-  </si>
-  <si>
-    <t>MEDH_15A</t>
-  </si>
-  <si>
-    <t>MEDH_15B</t>
-  </si>
-  <si>
-    <t>MEDH_20A</t>
-  </si>
-  <si>
-    <t>MEDH_20B</t>
-  </si>
-  <si>
-    <t>MEDH_22A</t>
-  </si>
-  <si>
-    <t>MEDH_22B</t>
-  </si>
-  <si>
-    <t>MEDH_24A</t>
-  </si>
-  <si>
-    <t>MEDH_24B</t>
-  </si>
-  <si>
     <t>Time_hrs</t>
   </si>
   <si>
@@ -108,12 +70,111 @@
   </si>
   <si>
     <t>Ordered</t>
+  </si>
+  <si>
+    <t>Sample_ID</t>
+  </si>
+  <si>
+    <t>MEDH_5m_180223</t>
+  </si>
+  <si>
+    <t>MEDH_10m_180223</t>
+  </si>
+  <si>
+    <t>MEDH_15m_180223</t>
+  </si>
+  <si>
+    <t>MEDH_20m_180223</t>
+  </si>
+  <si>
+    <t>MEDH_22m_180223</t>
+  </si>
+  <si>
+    <t>MEDH_23m_180223</t>
+  </si>
+  <si>
+    <t>MEDH_5m_180226</t>
+  </si>
+  <si>
+    <t>MEDH_10m_180226</t>
+  </si>
+  <si>
+    <t>MEDH_15m_180226</t>
+  </si>
+  <si>
+    <t>MEDH_20m_180226</t>
+  </si>
+  <si>
+    <t>MEDH_22m_180226</t>
+  </si>
+  <si>
+    <t>MEDH_23m_180226</t>
+  </si>
+  <si>
+    <t>Incub2_5A_180223</t>
+  </si>
+  <si>
+    <t>Incub2_5B_180223</t>
+  </si>
+  <si>
+    <t>Incub2_10A_180223</t>
+  </si>
+  <si>
+    <t>Incub2_10B_180223</t>
+  </si>
+  <si>
+    <t>Incub2_15A_180223</t>
+  </si>
+  <si>
+    <t>Reading_A</t>
+  </si>
+  <si>
+    <t>Ammonia_concentratioin</t>
+  </si>
+  <si>
+    <t>MEDH_5_A</t>
+  </si>
+  <si>
+    <t>MEDH_5_B</t>
+  </si>
+  <si>
+    <t>MEDH_10_A</t>
+  </si>
+  <si>
+    <t>MEDH_15_A</t>
+  </si>
+  <si>
+    <t>MEDH_20_A</t>
+  </si>
+  <si>
+    <t>MEDH_22_A</t>
+  </si>
+  <si>
+    <t>MEDH_24_A</t>
+  </si>
+  <si>
+    <t>MEDH_10_B</t>
+  </si>
+  <si>
+    <t>MEDH_15_B</t>
+  </si>
+  <si>
+    <t>MEDH_20_B</t>
+  </si>
+  <si>
+    <t>MEDH_22_B</t>
+  </si>
+  <si>
+    <t>MEDH_24_B</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -137,7 +198,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -145,11 +206,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -158,8 +234,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -297,7 +375,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$I$35:$I$40</c:f>
+              <c:f>'180227_results'!$C$29:$C$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -324,7 +402,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$J$35:$J$40</c:f>
+              <c:f>'180227_results'!$D$29:$D$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -378,162 +456,126 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$25</c:f>
+              <c:f>'180227_results'!$D$8:$D$25</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="24"/>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>0.32</c:v>
+                  <c:v>0.261</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0.67</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.346</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.232</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.438</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.675</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.262</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.349</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>0.319</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="9">
                   <c:v>0.408</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.327</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.357</c:v>
-                </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="10">
                   <c:v>0.264</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.332</c:v>
-                </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="11">
                   <c:v>0.33</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="12">
                   <c:v>0.338</c:v>
                 </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.261</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.67</c:v>
-                </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="13">
                   <c:v>0.43</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="14">
                   <c:v>0.758</c:v>
                 </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.346</c:v>
-                </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>0.31</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.232</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>0.455</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.438</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.675</c:v>
-                </c:pt>
-                <c:pt idx="19">
                   <c:v>0.358</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0.313</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0.262</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0.349</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>0.333</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$25</c:f>
+              <c:f>'180227_results'!$E$8:$E$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="24"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>22.95434</c:v>
+                  <c:v>18.595892</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>48.80954000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>24.875012</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.453604</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>31.671236</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>49.1789</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>18.669764</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>25.096628</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>22.880468</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="9">
                   <c:v>29.455076</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>23.471444</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>25.687604</c:v>
-                </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="10">
                   <c:v>18.817508</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>23.840804</c:v>
-                </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="11">
                   <c:v>23.69306</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="12">
                   <c:v>24.284036</c:v>
                 </c:pt>
-                <c:pt idx="9">
-                  <c:v>18.595892</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>48.80954000000001</c:v>
-                </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="13">
                   <c:v>31.08026</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="14">
                   <c:v>55.310276</c:v>
                 </c:pt>
-                <c:pt idx="13">
-                  <c:v>24.875012</c:v>
-                </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>22.21562</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>16.453604</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>32.92706</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>31.671236</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>49.1789</c:v>
-                </c:pt>
-                <c:pt idx="19">
                   <c:v>25.761476</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>22.437236</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>18.669764</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>25.096628</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>23.914676</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -548,11 +590,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-378388512"/>
-        <c:axId val="-283600608"/>
+        <c:axId val="1615236304"/>
+        <c:axId val="1617609328"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-378388512"/>
+        <c:axId val="1615236304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -664,12 +706,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-283600608"/>
+        <c:crossAx val="1617609328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-283600608"/>
+        <c:axId val="1617609328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -750,6 +792,7 @@
             </a:p>
           </c:txPr>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -786,7 +829,475 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-378388512"/>
+        <c:crossAx val="1615236304"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-CA"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="31750" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'180228_results'!$B$2:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.063</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.145</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.292</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.572</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'180228_results'!$C$2:$C$7</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.125</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1615730912"/>
+        <c:axId val="1615745920"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1615730912"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Wavelength(A)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1615745920"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1615745920"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Ammonia Concentration</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" baseline="0"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1615730912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -875,7 +1386,563 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1409,6 +2476,41 @@
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>806174</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>115326</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>408609</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>192315</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1689,10 +2791,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J40"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView zoomScale="124" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1704,580 +2806,882 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="E1" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
-        <v>22</v>
+      <c r="A2" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>4</v>
+        <v>34</v>
       </c>
       <c r="C2" s="3">
         <v>69</v>
       </c>
-      <c r="D2" s="4">
-        <v>0.32</v>
+      <c r="D2" s="7">
+        <v>0.313</v>
       </c>
       <c r="E2">
         <f>(73.872*D2)-0.6847</f>
-        <v>22.954340000000002</v>
+        <v>22.437236000000002</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="str">
+      <c r="A3" s="4" t="str">
         <f>A2</f>
         <v>2/16/2018</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="C3" s="3">
-        <v>92</v>
-      </c>
-      <c r="D3" s="4">
-        <v>0.31900000000000001</v>
+        <v>69</v>
+      </c>
+      <c r="D3" s="7">
+        <v>0.33300000000000002</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E25" si="0">(73.872*D3)-0.6847</f>
-        <v>22.880468</v>
+        <f>(73.872*D3)-0.6847</f>
+        <v>23.914676000000004</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="str">
-        <f t="shared" ref="A4:A25" si="1">A3</f>
+      <c r="A4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="3">
+        <v>69</v>
+      </c>
+      <c r="D4" s="7">
+        <v>0.32</v>
+      </c>
+      <c r="E4">
+        <f>(73.872*D4)-0.6847</f>
+        <v>22.954340000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="str">
+        <f>A4</f>
         <v>2/16/2018</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="3">
-        <v>92</v>
-      </c>
-      <c r="D4" s="4">
-        <v>0.40799999999999997</v>
-      </c>
-      <c r="E4">
-        <f t="shared" si="0"/>
-        <v>29.455075999999998</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>2/16/2018</v>
-      </c>
       <c r="B5" s="3" t="s">
-        <v>5</v>
+        <v>41</v>
       </c>
       <c r="C5" s="3">
         <v>69</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="7">
         <v>0.32700000000000001</v>
       </c>
       <c r="E5">
-        <f t="shared" si="0"/>
+        <f>(73.872*D5)-0.6847</f>
         <v>23.471444000000002</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="str">
-        <f t="shared" si="1"/>
+      <c r="A6" s="4" t="str">
+        <f>A5</f>
         <v>2/16/2018</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="C6" s="3">
         <v>69</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="7">
         <v>0.35699999999999998</v>
       </c>
       <c r="E6">
-        <f t="shared" si="0"/>
+        <f>(73.872*D6)-0.6847</f>
         <v>25.687604</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="str">
-        <f t="shared" si="1"/>
+      <c r="A7" s="4" t="str">
+        <f>A6</f>
         <v>2/16/2018</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="C7" s="3">
-        <v>92</v>
-      </c>
-      <c r="D7" s="4">
-        <v>0.26400000000000001</v>
+        <v>69</v>
+      </c>
+      <c r="D7" s="7">
+        <v>0.33200000000000002</v>
       </c>
       <c r="E7">
-        <f t="shared" si="0"/>
-        <v>18.817508</v>
+        <f>(73.872*D7)-0.6847</f>
+        <v>23.840804000000002</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="str">
-        <f t="shared" si="1"/>
+      <c r="A8" s="4" t="str">
+        <f>A7</f>
         <v>2/16/2018</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="3">
+      <c r="B8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="1">
         <v>69</v>
       </c>
-      <c r="D8" s="4">
-        <v>0.33200000000000002</v>
+      <c r="D8" s="6">
+        <v>0.26100000000000001</v>
       </c>
       <c r="E8">
-        <f t="shared" si="0"/>
-        <v>23.840804000000002</v>
+        <f>(73.872*D8)-0.6847</f>
+        <v>18.595892000000003</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="str">
-        <f t="shared" si="1"/>
+      <c r="A9" s="4" t="str">
+        <f>A8</f>
         <v>2/16/2018</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="3">
-        <v>92</v>
-      </c>
-      <c r="D9" s="4">
-        <v>0.33</v>
+      <c r="B9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="1">
+        <v>69</v>
+      </c>
+      <c r="D9" s="6">
+        <v>0.67</v>
       </c>
       <c r="E9">
-        <f t="shared" si="0"/>
-        <v>23.693060000000003</v>
+        <f>(73.872*D9)-0.6847</f>
+        <v>48.809540000000005</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="str">
-        <f t="shared" si="1"/>
+      <c r="A10" s="4" t="str">
+        <f>A9</f>
         <v>2/16/2018</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="C10" s="1">
-        <v>92</v>
-      </c>
-      <c r="D10" s="2">
-        <v>0.33800000000000002</v>
+        <v>69</v>
+      </c>
+      <c r="D10" s="6">
+        <v>0.34599999999999997</v>
       </c>
       <c r="E10">
-        <f t="shared" si="0"/>
-        <v>24.284036000000004</v>
+        <f>(73.872*D10)-0.6847</f>
+        <v>24.875011999999998</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="str">
-        <f t="shared" si="1"/>
+      <c r="A11" s="4" t="str">
+        <f>A10</f>
         <v>2/16/2018</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>8</v>
+        <v>44</v>
       </c>
       <c r="C11" s="1">
         <v>69</v>
       </c>
-      <c r="D11" s="2">
-        <v>0.26100000000000001</v>
+      <c r="D11" s="6">
+        <v>0.23200000000000001</v>
       </c>
       <c r="E11">
-        <f t="shared" si="0"/>
-        <v>18.595892000000003</v>
+        <f>(73.872*D11)-0.6847</f>
+        <v>16.453604000000002</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="str">
-        <f t="shared" si="1"/>
+      <c r="A12" s="4" t="str">
+        <f>A11</f>
         <v>2/16/2018</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>9</v>
+        <v>40</v>
       </c>
       <c r="C12" s="1">
         <v>69</v>
       </c>
-      <c r="D12" s="2">
-        <v>0.67</v>
+      <c r="D12" s="6">
+        <v>0.438</v>
       </c>
       <c r="E12">
-        <f t="shared" si="0"/>
-        <v>48.809540000000005</v>
+        <f>(73.872*D12)-0.6847</f>
+        <v>31.671236</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="5" t="str">
-        <f t="shared" si="1"/>
+      <c r="A13" s="4" t="str">
+        <f>A12</f>
         <v>2/16/2018</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>9</v>
+        <v>45</v>
       </c>
       <c r="C13" s="1">
+        <v>69</v>
+      </c>
+      <c r="D13" s="6">
+        <v>0.67500000000000004</v>
+      </c>
+      <c r="E13">
+        <f>(73.872*D13)-0.6847</f>
+        <v>49.178900000000006</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="str">
+        <f>A25</f>
+        <v>2/16/2018</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="3">
         <v>92</v>
       </c>
-      <c r="D13" s="2">
-        <v>0.43</v>
-      </c>
-      <c r="E13">
-        <f t="shared" si="0"/>
-        <v>31.080259999999999</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="5" t="str">
-        <f t="shared" si="1"/>
+      <c r="D14" s="7">
+        <v>0.26200000000000001</v>
+      </c>
+      <c r="E14">
+        <f>(73.872*D14)-0.6847</f>
+        <v>18.669764000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="str">
+        <f>A14</f>
         <v>2/16/2018</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="1">
+      <c r="B15" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="3">
         <v>92</v>
       </c>
-      <c r="D14" s="2">
-        <v>0.75800000000000001</v>
-      </c>
-      <c r="E14">
-        <f t="shared" si="0"/>
-        <v>55.310276000000002</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="5" t="str">
-        <f t="shared" si="1"/>
+      <c r="D15" s="7">
+        <v>0.34899999999999998</v>
+      </c>
+      <c r="E15">
+        <f>(73.872*D15)-0.6847</f>
+        <v>25.096627999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="str">
+        <f>A3</f>
         <v>2/16/2018</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="1">
-        <v>69</v>
-      </c>
-      <c r="D15" s="2">
-        <v>0.34599999999999997</v>
-      </c>
-      <c r="E15">
-        <f t="shared" si="0"/>
-        <v>24.875011999999998</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="5" t="str">
-        <f t="shared" si="1"/>
+      <c r="B16" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="3">
+        <v>92</v>
+      </c>
+      <c r="D16" s="7">
+        <v>0.31900000000000001</v>
+      </c>
+      <c r="E16">
+        <f>(73.872*D16)-0.6847</f>
+        <v>22.880468</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="str">
+        <f>A16</f>
         <v>2/16/2018</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" s="1">
+      <c r="B17" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" s="3">
         <v>92</v>
       </c>
-      <c r="D16" s="2">
-        <v>0.31</v>
-      </c>
-      <c r="E16">
-        <f t="shared" si="0"/>
-        <v>22.215620000000001</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="5" t="str">
-        <f t="shared" si="1"/>
+      <c r="D17" s="7">
+        <v>0.40799999999999997</v>
+      </c>
+      <c r="E17">
+        <f>(73.872*D17)-0.6847</f>
+        <v>29.455075999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="str">
+        <f>A17</f>
         <v>2/16/2018</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C17" s="1">
-        <v>69</v>
-      </c>
-      <c r="D17" s="2">
-        <v>0.23200000000000001</v>
-      </c>
-      <c r="E17">
-        <f t="shared" si="0"/>
-        <v>16.453604000000002</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="5" t="str">
-        <f t="shared" si="1"/>
+      <c r="B18" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="3">
+        <v>92</v>
+      </c>
+      <c r="D18" s="7">
+        <v>0.26400000000000001</v>
+      </c>
+      <c r="E18">
+        <f>(73.872*D18)-0.6847</f>
+        <v>18.817508</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="str">
+        <f>A18</f>
         <v>2/16/2018</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C18" s="1">
+      <c r="B19" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="3">
         <v>92</v>
       </c>
-      <c r="D18" s="2">
-        <v>0.45500000000000002</v>
-      </c>
-      <c r="E18">
-        <f t="shared" si="0"/>
-        <v>32.927060000000004</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="5" t="str">
-        <f t="shared" si="1"/>
+      <c r="D19" s="7">
+        <v>0.33</v>
+      </c>
+      <c r="E19">
+        <f>(73.872*D19)-0.6847</f>
+        <v>23.693060000000003</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="str">
+        <f>A19</f>
         <v>2/16/2018</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C19" s="1">
-        <v>69</v>
-      </c>
-      <c r="D19" s="2">
-        <v>0.438</v>
-      </c>
-      <c r="E19">
-        <f t="shared" si="0"/>
-        <v>31.671236</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="5" t="str">
-        <f t="shared" si="1"/>
+      <c r="B20" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="1">
+        <v>92</v>
+      </c>
+      <c r="D20" s="6">
+        <v>0.33800000000000002</v>
+      </c>
+      <c r="E20">
+        <f>(73.872*D20)-0.6847</f>
+        <v>24.284036000000004</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="str">
+        <f>A20</f>
         <v>2/16/2018</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C20" s="1">
-        <v>69</v>
-      </c>
-      <c r="D20" s="2">
-        <v>0.67500000000000004</v>
-      </c>
-      <c r="E20">
-        <f t="shared" si="0"/>
-        <v>49.178900000000006</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>2/16/2018</v>
-      </c>
       <c r="B21" s="1" t="s">
-        <v>13</v>
+        <v>43</v>
       </c>
       <c r="C21" s="1">
         <v>92</v>
       </c>
-      <c r="D21" s="2">
+      <c r="D21" s="6">
+        <v>0.43</v>
+      </c>
+      <c r="E21">
+        <f>(73.872*D21)-0.6847</f>
+        <v>31.080259999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="str">
+        <f>A21</f>
+        <v>2/16/2018</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="1">
+        <v>92</v>
+      </c>
+      <c r="D22" s="6">
+        <v>0.75800000000000001</v>
+      </c>
+      <c r="E22">
+        <f>(73.872*D22)-0.6847</f>
+        <v>55.310276000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="str">
+        <f>A22</f>
+        <v>2/16/2018</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" s="1">
+        <v>92</v>
+      </c>
+      <c r="D23" s="6">
+        <v>0.31</v>
+      </c>
+      <c r="E23">
+        <f>(73.872*D23)-0.6847</f>
+        <v>22.215620000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="str">
+        <f>A23</f>
+        <v>2/16/2018</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" s="1">
+        <v>92</v>
+      </c>
+      <c r="D24" s="6">
+        <v>0.45500000000000002</v>
+      </c>
+      <c r="E24">
+        <f>(73.872*D24)-0.6847</f>
+        <v>32.927060000000004</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="str">
+        <f>A24</f>
+        <v>2/16/2018</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C25" s="1">
+        <v>92</v>
+      </c>
+      <c r="D25" s="6">
         <v>0.35799999999999998</v>
       </c>
-      <c r="E21">
-        <f t="shared" si="0"/>
+      <c r="E25">
+        <f>(73.872*D25)-0.6847</f>
         <v>25.761475999999998</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>2/16/2018</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C22" s="3">
-        <v>69</v>
-      </c>
-      <c r="D22" s="4">
-        <v>0.313</v>
-      </c>
-      <c r="E22">
-        <f t="shared" si="0"/>
-        <v>22.437236000000002</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>2/16/2018</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C23" s="3">
-        <v>92</v>
-      </c>
-      <c r="D23" s="4">
-        <v>0.26200000000000001</v>
-      </c>
-      <c r="E23">
-        <f t="shared" si="0"/>
-        <v>18.669764000000001</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>2/16/2018</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C24" s="3">
-        <v>92</v>
-      </c>
-      <c r="D24" s="4">
-        <v>0.34899999999999998</v>
-      </c>
-      <c r="E24">
-        <f t="shared" si="0"/>
-        <v>25.096627999999999</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>2/16/2018</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C25" s="3">
-        <v>69</v>
-      </c>
-      <c r="D25" s="4">
-        <v>0.33300000000000002</v>
-      </c>
-      <c r="E25">
-        <f t="shared" si="0"/>
-        <v>23.914676000000004</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
     </row>
-    <row r="34" spans="7:10" x14ac:dyDescent="0.2">
-      <c r="H34" t="s">
-        <v>24</v>
-      </c>
-      <c r="I34" t="s">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28" t="s">
+        <v>12</v>
+      </c>
+      <c r="D28" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B29" s="1">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" s="1">
+        <v>50</v>
+      </c>
+      <c r="C30">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="D30">
+        <v>3.125</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" s="1">
+        <v>3.125</v>
+      </c>
+      <c r="C31">
+        <v>0.13700000000000001</v>
+      </c>
+      <c r="D31">
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B32" s="1">
+        <v>12.5</v>
+      </c>
+      <c r="C32">
+        <v>0.189</v>
+      </c>
+      <c r="D32">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B33" s="1">
+        <v>6.25</v>
+      </c>
+      <c r="C33">
+        <v>0.32100000000000001</v>
+      </c>
+      <c r="D33">
         <v>25</v>
       </c>
-      <c r="J34" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="35" spans="7:10" x14ac:dyDescent="0.2">
-      <c r="G35" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H35" s="1">
-        <v>0</v>
-      </c>
-      <c r="I35">
-        <v>0</v>
-      </c>
-      <c r="J35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="7:10" x14ac:dyDescent="0.2">
-      <c r="G36" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H36" s="1">
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B34" s="1">
+        <v>25</v>
+      </c>
+      <c r="C34">
+        <v>0.68799999999999994</v>
+      </c>
+      <c r="D34">
         <v>50</v>
       </c>
-      <c r="I36">
-        <v>3.2000000000000001E-2</v>
-      </c>
-      <c r="J36">
-        <v>3.125</v>
-      </c>
-    </row>
-    <row r="37" spans="7:10" x14ac:dyDescent="0.2">
-      <c r="G37" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H37" s="1">
-        <v>3.125</v>
-      </c>
-      <c r="I37">
-        <v>0.13700000000000001</v>
-      </c>
-      <c r="J37">
-        <v>6.25</v>
-      </c>
-    </row>
-    <row r="38" spans="7:10" x14ac:dyDescent="0.2">
-      <c r="G38" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H38" s="1">
-        <v>12.5</v>
-      </c>
-      <c r="I38">
-        <v>0.189</v>
-      </c>
-      <c r="J38">
-        <v>12.5</v>
-      </c>
-    </row>
-    <row r="39" spans="7:10" x14ac:dyDescent="0.2">
-      <c r="G39" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H39" s="1">
-        <v>6.25</v>
-      </c>
-      <c r="I39">
-        <v>0.32100000000000001</v>
-      </c>
-      <c r="J39">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="40" spans="7:10" x14ac:dyDescent="0.2">
-      <c r="G40" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H40" s="1">
-        <v>25</v>
-      </c>
-      <c r="I40">
-        <v>0.68799999999999994</v>
-      </c>
-      <c r="J40">
-        <v>50</v>
-      </c>
     </row>
   </sheetData>
-  <sortState ref="A2:D40">
-    <sortCondition ref="B1"/>
+  <sortState ref="A2:E25">
+    <sortCondition ref="C2:C25"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="160" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="6">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="6">
+        <v>6.3E-2</v>
+      </c>
+      <c r="C3" s="2">
+        <v>3.125</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="6">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="C4" s="2">
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="6">
+        <v>0.29199999999999998</v>
+      </c>
+      <c r="C5" s="2">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="6">
+        <v>0.57199999999999995</v>
+      </c>
+      <c r="C6" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="6">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="C7" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="6">
+        <v>-2E-3</v>
+      </c>
+      <c r="C8" s="2">
+        <f>43.409*B8+0.07</f>
+        <v>-1.6818E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="6">
+        <v>-1.0999999999999999E-2</v>
+      </c>
+      <c r="C9" s="2">
+        <f t="shared" ref="C9:C24" si="0">43.409*B9+0.07</f>
+        <v>-0.40749899999999994</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="6">
+        <v>-4.2999999999999997E-2</v>
+      </c>
+      <c r="C10" s="2">
+        <f t="shared" si="0"/>
+        <v>-1.7965869999999997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="6">
+        <v>-0.1</v>
+      </c>
+      <c r="C11" s="2">
+        <f t="shared" si="0"/>
+        <v>-4.2709000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="6">
+        <v>-6.0000000000000001E-3</v>
+      </c>
+      <c r="C12" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.19045400000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="6">
+        <v>-5.0000000000000001E-3</v>
+      </c>
+      <c r="C13" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.14704499999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="6">
+        <v>-2.1000000000000001E-2</v>
+      </c>
+      <c r="C14" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.84158899999999992</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="6">
+        <v>-0.01</v>
+      </c>
+      <c r="C15" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.36408999999999997</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="6">
+        <v>-0.04</v>
+      </c>
+      <c r="C16" s="2">
+        <f t="shared" si="0"/>
+        <v>-1.6663599999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="6">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="C17" s="2">
+        <f t="shared" si="0"/>
+        <v>0.41727200000000003</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="6">
+        <v>-8.0000000000000002E-3</v>
+      </c>
+      <c r="C18" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.27727200000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="6">
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="C19" s="2">
+        <f t="shared" si="0"/>
+        <v>3.8899919999999995</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" s="6">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="C20" s="2">
+        <f t="shared" si="0"/>
+        <v>9.8370250000000006</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="6">
+        <v>0.115</v>
+      </c>
+      <c r="C21" s="2">
+        <f t="shared" si="0"/>
+        <v>5.0620350000000007</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" s="6">
+        <v>0.17</v>
+      </c>
+      <c r="C22" s="2">
+        <f t="shared" si="0"/>
+        <v>7.4495300000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" s="6">
+        <v>0.187</v>
+      </c>
+      <c r="C23" s="2">
+        <f t="shared" si="0"/>
+        <v>8.1874830000000003</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24" s="6">
+        <v>0.14399999999999999</v>
+      </c>
+      <c r="C24" s="2">
+        <f t="shared" si="0"/>
+        <v>6.3208959999999994</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>